<commit_message>
new works updated on task evaluation sheet
</commit_message>
<xml_diff>
--- a/All Tasks/Task Evaluation/Task Evaluation Sheet_Jakia Rahman_Intern(MIS).xlsx
+++ b/All Tasks/Task Evaluation/Task Evaluation Sheet_Jakia Rahman_Intern(MIS).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Internship\SQA-Internship-Progress-in-HPL\All Tasks\Task Evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F7FD23B-92AC-4F39-99E1-7087BB65A57F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{161DE202-1E48-4631-A492-659E4084A77F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="149">
   <si>
     <t>Task No.</t>
   </si>
@@ -395,21 +395,9 @@
     <t>SAP Product Allocation Module</t>
   </si>
   <si>
-    <t>HCL Website Development</t>
-  </si>
-  <si>
     <t>1. HTML5
 2. Tailwind CSS v3.0
 3. Javascript</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Updated website sections including Footer, Header, History, Messages from Leaders, Service, Contact, News &amp; Blogs.
-2. Learned layout design, content placement, and consistent styling.
-3. Practiced iterative content updates and review </t>
-  </si>
-  <si>
-    <t>10/15/2025
-(Ongoing)</t>
   </si>
   <si>
     <t>Module No.</t>
@@ -706,14 +694,68 @@
     <t xml:space="preserve">Healthcare Pharmaceuticals Limited </t>
   </si>
   <si>
-    <t>Internship Task Summary (1st July – 10th October 2025)</t>
+    <t>Internship Task Summary (1st July – 10th November 2025)</t>
+  </si>
+  <si>
+    <t>1. Started Pulse App Regression Testing for v2.2.5.  - Verified app stability and functionality for v3.0.0, focusing on the new “Saved Order” feature to ensure proper performance and integration.</t>
+  </si>
+  <si>
+    <t>Data Base Testing</t>
+  </si>
+  <si>
+    <t>1. Fundamentals of Database Testing</t>
+  </si>
+  <si>
+    <t>Tools and Technologies</t>
+  </si>
+  <si>
+    <t>1. Overview of QA Tools and Technologies</t>
+  </si>
+  <si>
+    <t>Project Week 2</t>
+  </si>
+  <si>
+    <t>1. Updated website sections including Footer, Header, History, Messages from Leaders, Service, Contact, News &amp; Blogs.
+2. Learned layout design, content placement, and consistent styling.</t>
+  </si>
+  <si>
+    <t>HCL Website Development (hclapibd.com)</t>
+  </si>
+  <si>
+    <t>1. New Project Implementation (Tools - Playwright, Javascript, Allure Report)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Website hosted on </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>hclapibd.com</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> via cPanel.
+2. Currently working on new updates — making the site fully responsive, adding new content, and implementing fresh design improvements.
+3. Managing version updates directly through cPanel File Manager.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -774,6 +816,13 @@
       <name val="Cambria"/>
       <family val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -801,7 +850,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -837,11 +886,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -946,6 +1021,18 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1230,10 +1317,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J273"/>
+  <dimension ref="A1:J269"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A78" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72:G87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1249,21 +1336,21 @@
   <sheetData>
     <row r="1" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" s="30" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D1" s="30"/>
       <c r="E1" s="30"/>
     </row>
     <row r="2" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="31" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D2" s="31"/>
       <c r="E2" s="31"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C3" s="32" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D3" s="32"/>
       <c r="E3" s="32"/>
@@ -1600,7 +1687,7 @@
         <v>59</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D23" s="18" t="s">
         <v>54</v>
@@ -1626,7 +1713,7 @@
         <v>60</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D24" s="18" t="s">
         <v>54</v>
@@ -1866,15 +1953,29 @@
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
-      <c r="H35" s="5"/>
+    <row r="35" spans="1:10" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="37">
+        <v>15</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="D35" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="E35" s="20">
+        <v>45967</v>
+      </c>
+      <c r="F35" s="20">
+        <v>45970</v>
+      </c>
+      <c r="G35" s="20">
+        <v>45971</v>
+      </c>
+      <c r="H35" s="7"/>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
     </row>
@@ -1902,13 +2003,9 @@
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
     </row>
-    <row r="38" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="B38" s="21" t="s">
-        <v>134</v>
-      </c>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="12"/>
       <c r="E38" s="12"/>
@@ -1918,9 +2015,13 @@
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
     </row>
-    <row r="39" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="8"/>
-      <c r="B39" s="8"/>
+    <row r="39" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B39" s="21" t="s">
+        <v>131</v>
+      </c>
       <c r="C39" s="5"/>
       <c r="D39" s="12"/>
       <c r="E39" s="12"/>
@@ -1930,90 +2031,76 @@
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B40" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C40" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D40" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E40" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="F40" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="G40" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="H40" s="6"/>
+    <row r="40" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="8"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="5"/>
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
     </row>
-    <row r="41" spans="1:10" ht="71.25" x14ac:dyDescent="0.25">
-      <c r="A41" s="18">
-        <v>15</v>
-      </c>
-      <c r="B41" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="C41" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="D41" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="E41" s="20">
-        <v>45890</v>
-      </c>
-      <c r="F41" s="20">
-        <v>45890</v>
-      </c>
-      <c r="G41" s="20">
-        <v>45890</v>
-      </c>
-      <c r="H41" s="7"/>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F41" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G41" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H41" s="6"/>
       <c r="I41" s="5"/>
       <c r="J41" s="5"/>
     </row>
-    <row r="42" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" ht="57" x14ac:dyDescent="0.25">
       <c r="A42" s="18">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B42" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>67</v>
+        <v>33</v>
       </c>
       <c r="D42" s="18" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
       <c r="E42" s="20">
-        <v>45893</v>
+        <v>45890</v>
       </c>
       <c r="F42" s="20">
-        <v>45893</v>
+        <v>45890</v>
       </c>
       <c r="G42" s="20">
-        <v>45893</v>
+        <v>45890</v>
       </c>
       <c r="H42" s="7"/>
       <c r="I42" s="5"/>
       <c r="J42" s="5"/>
     </row>
-    <row r="43" spans="1:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B43" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C43" s="19" t="s">
         <v>67</v>
@@ -2022,57 +2109,71 @@
         <v>7</v>
       </c>
       <c r="E43" s="20">
-        <v>45894</v>
+        <v>45893</v>
       </c>
       <c r="F43" s="20">
-        <v>45894</v>
+        <v>45893</v>
       </c>
       <c r="G43" s="20">
-        <v>45894</v>
+        <v>45893</v>
       </c>
       <c r="H43" s="7"/>
       <c r="I43" s="5"/>
       <c r="J43" s="5"/>
     </row>
-    <row r="44" spans="1:10" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="18">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B44" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
       <c r="D44" s="18" t="s">
         <v>7</v>
       </c>
       <c r="E44" s="20">
-        <v>45876</v>
+        <v>45894</v>
       </c>
       <c r="F44" s="20">
-        <v>45876</v>
+        <v>45894</v>
       </c>
       <c r="G44" s="20">
-        <v>45876</v>
+        <v>45894</v>
       </c>
       <c r="H44" s="7"/>
       <c r="I44" s="5"/>
       <c r="J44" s="5"/>
     </row>
-    <row r="45" spans="1:10" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
-      <c r="B45" s="5"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
-      <c r="G45" s="12"/>
-      <c r="H45" s="5"/>
+    <row r="45" spans="1:10" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A45" s="18">
+        <v>18</v>
+      </c>
+      <c r="B45" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C45" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D45" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45" s="20">
+        <v>45876</v>
+      </c>
+      <c r="F45" s="20">
+        <v>45876</v>
+      </c>
+      <c r="G45" s="20">
+        <v>45876</v>
+      </c>
+      <c r="H45" s="7"/>
       <c r="I45" s="5"/>
       <c r="J45" s="5"/>
     </row>
-    <row r="46" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
@@ -2084,14 +2185,10 @@
       <c r="I46" s="5"/>
       <c r="J46" s="5"/>
     </row>
-    <row r="47" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="B47" s="33" t="s">
-        <v>93</v>
-      </c>
-      <c r="C47" s="33"/>
+    <row r="47" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="5"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
       <c r="D47" s="12"/>
       <c r="E47" s="12"/>
       <c r="F47" s="12"/>
@@ -2100,10 +2197,14 @@
       <c r="I47" s="5"/>
       <c r="J47" s="5"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="5"/>
-      <c r="B48" s="5"/>
-      <c r="C48" s="5"/>
+    <row r="48" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B48" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="C48" s="33"/>
       <c r="D48" s="12"/>
       <c r="E48" s="12"/>
       <c r="F48" s="12"/>
@@ -2113,181 +2214,177 @@
       <c r="J48" s="5"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B49" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C49" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D49" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E49" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="F49" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="G49" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="H49" s="6"/>
+      <c r="A49" s="5"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
+      <c r="H49" s="5"/>
       <c r="I49" s="5"/>
       <c r="J49" s="5"/>
     </row>
-    <row r="50" spans="1:10" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="18">
-        <v>19</v>
-      </c>
-      <c r="B50" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="C50" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="D50" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="E50" s="20">
-        <v>45845</v>
-      </c>
-      <c r="F50" s="20">
-        <v>45845</v>
-      </c>
-      <c r="G50" s="20">
-        <v>45911</v>
-      </c>
-      <c r="H50" s="7"/>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B50" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C50" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D50" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E50" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F50" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G50" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H50" s="6"/>
       <c r="I50" s="5"/>
       <c r="J50" s="5"/>
     </row>
-    <row r="51" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="18">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B51" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C51" s="19" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D51" s="18" t="s">
         <v>65</v>
       </c>
       <c r="E51" s="20">
-        <v>45908</v>
+        <v>45845</v>
       </c>
       <c r="F51" s="20">
-        <v>45908</v>
+        <v>45845</v>
       </c>
       <c r="G51" s="20">
-        <v>45908</v>
+        <v>45911</v>
       </c>
       <c r="H51" s="7"/>
       <c r="I51" s="5"/>
       <c r="J51" s="5"/>
     </row>
-    <row r="52" spans="1:10" ht="57" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="18">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B52" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C52" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D52" s="18" t="s">
         <v>65</v>
       </c>
       <c r="E52" s="20">
-        <v>45910</v>
+        <v>45908</v>
       </c>
       <c r="F52" s="20">
-        <v>45910</v>
+        <v>45908</v>
       </c>
       <c r="G52" s="20">
-        <v>45910</v>
+        <v>45908</v>
       </c>
       <c r="H52" s="7"/>
       <c r="I52" s="5"/>
       <c r="J52" s="5"/>
     </row>
-    <row r="53" spans="1:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A53" s="18">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B53" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C53" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D53" s="18" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="E53" s="20">
-        <v>45888</v>
+        <v>45910</v>
       </c>
       <c r="F53" s="20">
-        <v>45888</v>
+        <v>45910</v>
       </c>
       <c r="G53" s="20">
-        <v>45895</v>
+        <v>45910</v>
       </c>
       <c r="H53" s="7"/>
       <c r="I53" s="5"/>
       <c r="J53" s="5"/>
     </row>
-    <row r="54" spans="1:10" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="18">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B54" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C54" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D54" s="18" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="E54" s="20">
-        <v>45902</v>
+        <v>45888</v>
       </c>
       <c r="F54" s="20">
-        <v>45902</v>
+        <v>45888</v>
       </c>
       <c r="G54" s="20">
-        <v>45918</v>
+        <v>45895</v>
       </c>
       <c r="H54" s="7"/>
       <c r="I54" s="5"/>
       <c r="J54" s="5"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="5"/>
-      <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="12"/>
-      <c r="E55" s="12"/>
-      <c r="F55" s="12"/>
-      <c r="G55" s="12"/>
-      <c r="H55" s="5"/>
+    <row r="55" spans="1:10" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="18">
+        <v>23</v>
+      </c>
+      <c r="B55" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C55" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="D55" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="E55" s="20">
+        <v>45902</v>
+      </c>
+      <c r="F55" s="20">
+        <v>45902</v>
+      </c>
+      <c r="G55" s="20">
+        <v>45918</v>
+      </c>
+      <c r="H55" s="7"/>
       <c r="I55" s="5"/>
       <c r="J55" s="5"/>
     </row>
-    <row r="56" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="B56" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="C56" s="28"/>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="5"/>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
       <c r="D56" s="12"/>
       <c r="E56" s="12"/>
       <c r="F56" s="12"/>
@@ -2296,10 +2393,14 @@
       <c r="I56" s="5"/>
       <c r="J56" s="5"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" s="5"/>
-      <c r="B57" s="5"/>
-      <c r="C57" s="5"/>
+    <row r="57" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B57" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C57" s="28"/>
       <c r="D57" s="12"/>
       <c r="E57" s="12"/>
       <c r="F57" s="12"/>
@@ -2309,69 +2410,55 @@
       <c r="J57" s="5"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B58" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C58" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D58" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E58" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="F58" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="G58" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="H58" s="6"/>
+      <c r="A58" s="5"/>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="12"/>
+      <c r="E58" s="12"/>
+      <c r="F58" s="12"/>
+      <c r="G58" s="12"/>
+      <c r="H58" s="5"/>
       <c r="I58" s="5"/>
       <c r="J58" s="5"/>
     </row>
-    <row r="59" spans="1:10" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="18">
-        <v>24</v>
-      </c>
-      <c r="B59" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C59" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="D59" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="E59" s="20">
-        <v>45848</v>
-      </c>
-      <c r="F59" s="20">
-        <v>45848</v>
-      </c>
-      <c r="G59" s="20" t="s">
-        <v>135</v>
-      </c>
-      <c r="H59" s="7"/>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C59" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D59" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E59" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F59" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G59" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H59" s="6"/>
       <c r="I59" s="5"/>
       <c r="J59" s="5"/>
     </row>
-    <row r="60" spans="1:10" ht="57" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="18">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B60" s="18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C60" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D60" s="18" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="E60" s="20">
         <v>45848</v>
@@ -2379,48 +2466,62 @@
       <c r="F60" s="20">
         <v>45848</v>
       </c>
-      <c r="G60" s="20">
-        <v>45851</v>
+      <c r="G60" s="20" t="s">
+        <v>132</v>
       </c>
       <c r="H60" s="7"/>
       <c r="I60" s="5"/>
       <c r="J60" s="5"/>
     </row>
-    <row r="61" spans="1:10" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" ht="57" x14ac:dyDescent="0.25">
       <c r="A61" s="18">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B61" s="18" t="s">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="C61" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D61" s="18" t="s">
         <v>77</v>
       </c>
       <c r="E61" s="20">
+        <v>45848</v>
+      </c>
+      <c r="F61" s="20">
+        <v>45848</v>
+      </c>
+      <c r="G61" s="20">
         <v>45851</v>
-      </c>
-      <c r="F61" s="20">
-        <v>45851</v>
-      </c>
-      <c r="G61" s="20">
-        <v>45852</v>
       </c>
       <c r="H61" s="7"/>
       <c r="I61" s="5"/>
       <c r="J61" s="5"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62" s="5"/>
-      <c r="B62" s="5"/>
-      <c r="C62" s="5"/>
-      <c r="D62" s="12"/>
-      <c r="E62" s="12"/>
-      <c r="F62" s="12"/>
-      <c r="G62" s="12"/>
-      <c r="H62" s="5"/>
+    <row r="62" spans="1:10" ht="57" x14ac:dyDescent="0.25">
+      <c r="A62" s="18">
+        <v>26</v>
+      </c>
+      <c r="B62" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C62" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="D62" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="E62" s="20">
+        <v>45851</v>
+      </c>
+      <c r="F62" s="20">
+        <v>45851</v>
+      </c>
+      <c r="G62" s="20">
+        <v>45852</v>
+      </c>
+      <c r="H62" s="7"/>
       <c r="I62" s="5"/>
       <c r="J62" s="5"/>
     </row>
@@ -2436,14 +2537,10 @@
       <c r="I63" s="5"/>
       <c r="J63" s="5"/>
     </row>
-    <row r="64" spans="1:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="B64" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="C64" s="28"/>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" s="5"/>
+      <c r="B64" s="5"/>
+      <c r="C64" s="5"/>
       <c r="D64" s="12"/>
       <c r="E64" s="12"/>
       <c r="F64" s="12"/>
@@ -2452,10 +2549,14 @@
       <c r="I64" s="5"/>
       <c r="J64" s="5"/>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A65" s="5"/>
-      <c r="B65" s="5"/>
-      <c r="C65" s="5"/>
+    <row r="65" spans="1:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B65" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C65" s="28"/>
       <c r="D65" s="12"/>
       <c r="E65" s="12"/>
       <c r="F65" s="12"/>
@@ -2465,66 +2566,52 @@
       <c r="J65" s="5"/>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A66" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B66" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C66" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D66" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E66" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="F66" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="G66" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="H66" s="6"/>
+      <c r="A66" s="5"/>
+      <c r="B66" s="5"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="12"/>
+      <c r="E66" s="12"/>
+      <c r="F66" s="12"/>
+      <c r="G66" s="12"/>
+      <c r="H66" s="5"/>
       <c r="I66" s="5"/>
       <c r="J66" s="5"/>
     </row>
-    <row r="67" spans="1:10" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="18">
-        <v>27</v>
-      </c>
-      <c r="B67" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="C67" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="D67" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="E67" s="20">
-        <v>45875</v>
-      </c>
-      <c r="F67" s="20">
-        <v>45875</v>
-      </c>
-      <c r="G67" s="20">
-        <v>45883</v>
-      </c>
-      <c r="H67" s="7"/>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B67" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C67" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D67" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E67" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F67" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G67" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H67" s="6"/>
       <c r="I67" s="5"/>
       <c r="J67" s="5"/>
     </row>
-    <row r="68" spans="1:10" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="18">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B68" s="18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C68" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D68" s="18" t="s">
         <v>56</v>
@@ -2536,21 +2623,35 @@
         <v>45875</v>
       </c>
       <c r="G68" s="20">
-        <v>45880</v>
+        <v>45883</v>
       </c>
       <c r="H68" s="7"/>
       <c r="I68" s="5"/>
       <c r="J68" s="5"/>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A69" s="5"/>
-      <c r="B69" s="5"/>
-      <c r="C69" s="5"/>
-      <c r="D69" s="12"/>
-      <c r="E69" s="12"/>
-      <c r="F69" s="12"/>
-      <c r="G69" s="12"/>
-      <c r="H69" s="5"/>
+    <row r="69" spans="1:10" ht="57" x14ac:dyDescent="0.25">
+      <c r="A69" s="18">
+        <v>28</v>
+      </c>
+      <c r="B69" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C69" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="D69" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="E69" s="20">
+        <v>45875</v>
+      </c>
+      <c r="F69" s="20">
+        <v>45875</v>
+      </c>
+      <c r="G69" s="20">
+        <v>45880</v>
+      </c>
+      <c r="H69" s="7"/>
       <c r="I69" s="5"/>
       <c r="J69" s="5"/>
     </row>
@@ -2566,14 +2667,10 @@
       <c r="I70" s="5"/>
       <c r="J70" s="5"/>
     </row>
-    <row r="71" spans="1:10" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A71" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="B71" s="36" t="s">
-        <v>94</v>
-      </c>
-      <c r="C71" s="36"/>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71" s="5"/>
+      <c r="B71" s="5"/>
+      <c r="C71" s="5"/>
       <c r="D71" s="12"/>
       <c r="E71" s="12"/>
       <c r="F71" s="12"/>
@@ -2582,10 +2679,14 @@
       <c r="I71" s="5"/>
       <c r="J71" s="5"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A72" s="5"/>
-      <c r="B72" s="5"/>
-      <c r="C72" s="5"/>
+    <row r="72" spans="1:10" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A72" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="B72" s="36" t="s">
+        <v>94</v>
+      </c>
+      <c r="C72" s="36"/>
       <c r="D72" s="12"/>
       <c r="E72" s="12"/>
       <c r="F72" s="12"/>
@@ -2595,66 +2696,66 @@
       <c r="J72" s="5"/>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A73" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B73" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C73" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D73" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E73" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="F73" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="G73" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="H73" s="6"/>
+      <c r="A73" s="5"/>
+      <c r="B73" s="5"/>
+      <c r="C73" s="5"/>
+      <c r="D73" s="12"/>
+      <c r="E73" s="12"/>
+      <c r="F73" s="12"/>
+      <c r="G73" s="12"/>
+      <c r="H73" s="5"/>
       <c r="I73" s="5"/>
       <c r="J73" s="5"/>
     </row>
-    <row r="74" spans="1:10" ht="57" x14ac:dyDescent="0.25">
-      <c r="A74" s="18">
-        <v>29</v>
-      </c>
-      <c r="B74" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="C74" s="19" t="s">
-        <v>137</v>
-      </c>
-      <c r="D74" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="E74" s="20">
-        <v>45915</v>
-      </c>
-      <c r="F74" s="20">
-        <v>45915</v>
-      </c>
-      <c r="G74" s="20">
-        <v>45922</v>
-      </c>
-      <c r="H74" s="7"/>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A74" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B74" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C74" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D74" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E74" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F74" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G74" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H74" s="6"/>
       <c r="I74" s="5"/>
       <c r="J74" s="5"/>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A75" s="5"/>
-      <c r="B75" s="5"/>
-      <c r="C75" s="5"/>
-      <c r="D75" s="12"/>
-      <c r="E75" s="12"/>
-      <c r="F75" s="12"/>
-      <c r="G75" s="12"/>
-      <c r="H75" s="5"/>
+    <row r="75" spans="1:10" ht="57" x14ac:dyDescent="0.25">
+      <c r="A75" s="18">
+        <v>29</v>
+      </c>
+      <c r="B75" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="C75" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="D75" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="E75" s="20">
+        <v>45915</v>
+      </c>
+      <c r="F75" s="20">
+        <v>45915</v>
+      </c>
+      <c r="G75" s="20">
+        <v>45922</v>
+      </c>
+      <c r="H75" s="7"/>
       <c r="I75" s="5"/>
       <c r="J75" s="5"/>
     </row>
@@ -2682,14 +2783,10 @@
       <c r="I77" s="5"/>
       <c r="J77" s="5"/>
     </row>
-    <row r="78" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A78" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="B78" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="C78" s="28"/>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="5"/>
+      <c r="B78" s="5"/>
+      <c r="C78" s="5"/>
       <c r="D78" s="12"/>
       <c r="E78" s="12"/>
       <c r="F78" s="12"/>
@@ -2698,10 +2795,14 @@
       <c r="I78" s="5"/>
       <c r="J78" s="5"/>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A79" s="5"/>
-      <c r="B79" s="5"/>
-      <c r="C79" s="5"/>
+    <row r="79" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A79" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B79" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="C79" s="28"/>
       <c r="D79" s="12"/>
       <c r="E79" s="12"/>
       <c r="F79" s="12"/>
@@ -2711,66 +2812,52 @@
       <c r="J79" s="5"/>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A80" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B80" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C80" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D80" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E80" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="F80" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="G80" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="H80" s="6"/>
+      <c r="A80" s="5"/>
+      <c r="B80" s="5"/>
+      <c r="C80" s="5"/>
+      <c r="D80" s="12"/>
+      <c r="E80" s="12"/>
+      <c r="F80" s="12"/>
+      <c r="G80" s="12"/>
+      <c r="H80" s="5"/>
       <c r="I80" s="5"/>
       <c r="J80" s="5"/>
     </row>
-    <row r="81" spans="1:10" ht="85.5" x14ac:dyDescent="0.25">
-      <c r="A81" s="18">
-        <v>30</v>
-      </c>
-      <c r="B81" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C81" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="D81" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="E81" s="20">
-        <v>45918</v>
-      </c>
-      <c r="F81" s="20">
-        <v>45918</v>
-      </c>
-      <c r="G81" s="20">
-        <v>45930</v>
-      </c>
-      <c r="H81" s="7"/>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B81" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C81" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D81" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E81" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F81" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G81" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H81" s="6"/>
       <c r="I81" s="5"/>
       <c r="J81" s="5"/>
     </row>
-    <row r="82" spans="1:10" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A82" s="18">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B82" s="18" t="s">
-        <v>84</v>
+        <v>45</v>
       </c>
       <c r="C82" s="19" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="D82" s="18" t="s">
         <v>83</v>
@@ -2781,45 +2868,69 @@
       <c r="F82" s="20">
         <v>45918</v>
       </c>
-      <c r="G82" s="20" t="s">
-        <v>98</v>
+      <c r="G82" s="20">
+        <v>45930</v>
       </c>
       <c r="H82" s="7"/>
       <c r="I82" s="5"/>
       <c r="J82" s="5"/>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A83" s="5"/>
-      <c r="B83" s="5"/>
-      <c r="C83" s="5"/>
-      <c r="D83" s="12"/>
-      <c r="E83" s="12"/>
-      <c r="F83" s="12"/>
-      <c r="G83" s="12"/>
-      <c r="H83" s="5"/>
+    <row r="83" spans="1:10" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="18">
+        <v>31</v>
+      </c>
+      <c r="B83" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C83" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="D83" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="E83" s="20">
+        <v>45918</v>
+      </c>
+      <c r="F83" s="20">
+        <v>45918</v>
+      </c>
+      <c r="G83" s="20">
+        <v>45940</v>
+      </c>
+      <c r="H83" s="7"/>
       <c r="I83" s="5"/>
       <c r="J83" s="5"/>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A84" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="B84" s="5"/>
-      <c r="C84" s="5"/>
-      <c r="D84" s="12"/>
-      <c r="E84" s="12"/>
-      <c r="F84" s="12"/>
-      <c r="G84" s="12"/>
-      <c r="H84" s="5"/>
+    <row r="84" spans="1:10" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="18">
+        <v>32</v>
+      </c>
+      <c r="B84" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C84" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="D84" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="E84" s="20">
+        <v>45918</v>
+      </c>
+      <c r="F84" s="20">
+        <v>45919</v>
+      </c>
+      <c r="G84" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="H84" s="7"/>
       <c r="I84" s="5"/>
       <c r="J84" s="5"/>
     </row>
-    <row r="85" spans="1:10" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="B85" s="34"/>
-      <c r="C85" s="23"/>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="5"/>
+      <c r="B85" s="5"/>
+      <c r="C85" s="5"/>
       <c r="D85" s="12"/>
       <c r="E85" s="12"/>
       <c r="F85" s="12"/>
@@ -2829,7 +2940,9 @@
       <c r="J85" s="5"/>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A86" s="5"/>
+      <c r="A86" s="24" t="s">
+        <v>85</v>
+      </c>
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
       <c r="D86" s="12"/>
@@ -2840,10 +2953,12 @@
       <c r="I86" s="5"/>
       <c r="J86" s="5"/>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A87" s="5"/>
-      <c r="B87" s="5"/>
-      <c r="C87" s="5"/>
+    <row r="87" spans="1:10" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="B87" s="34"/>
+      <c r="C87" s="23"/>
       <c r="D87" s="12"/>
       <c r="E87" s="12"/>
       <c r="F87" s="12"/>
@@ -2852,14 +2967,10 @@
       <c r="I87" s="5"/>
       <c r="J87" s="5"/>
     </row>
-    <row r="88" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A88" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="B88" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="C88" s="28"/>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="5"/>
+      <c r="B88" s="5"/>
+      <c r="C88" s="5"/>
       <c r="D88" s="12"/>
       <c r="E88" s="12"/>
       <c r="F88" s="12"/>
@@ -2880,142 +2991,142 @@
       <c r="I89" s="5"/>
       <c r="J89" s="5"/>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A90" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B90" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C90" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D90" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E90" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="F90" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="G90" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="H90" s="6"/>
+    <row r="90" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A90" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B90" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="C90" s="28"/>
+      <c r="D90" s="12"/>
+      <c r="E90" s="12"/>
+      <c r="F90" s="12"/>
+      <c r="G90" s="12"/>
+      <c r="H90" s="5"/>
       <c r="I90" s="5"/>
       <c r="J90" s="5"/>
     </row>
-    <row r="91" spans="1:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="18">
-        <v>32</v>
-      </c>
-      <c r="B91" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="C91" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="D91" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="E91" s="20">
-        <v>45846</v>
-      </c>
-      <c r="F91" s="20">
-        <v>45846</v>
-      </c>
-      <c r="G91" s="20">
-        <v>45859</v>
-      </c>
-      <c r="H91" s="7"/>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="5"/>
+      <c r="B91" s="5"/>
+      <c r="C91" s="5"/>
+      <c r="D91" s="12"/>
+      <c r="E91" s="12"/>
+      <c r="F91" s="12"/>
+      <c r="G91" s="12"/>
+      <c r="H91" s="5"/>
       <c r="I91" s="5"/>
       <c r="J91" s="5"/>
     </row>
-    <row r="92" spans="1:10" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A92" s="18">
-        <v>33</v>
-      </c>
-      <c r="B92" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="C92" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="D92" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="E92" s="20">
-        <v>45862</v>
-      </c>
-      <c r="F92" s="20">
-        <v>45862</v>
-      </c>
-      <c r="G92" s="20">
-        <v>45862</v>
-      </c>
-      <c r="H92" s="7"/>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B92" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C92" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D92" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E92" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F92" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G92" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H92" s="6"/>
       <c r="I92" s="5"/>
       <c r="J92" s="5"/>
     </row>
-    <row r="93" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="18">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B93" s="18" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C93" s="19" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D93" s="18" t="s">
         <v>7</v>
       </c>
       <c r="E93" s="20">
-        <v>45888</v>
+        <v>45846</v>
       </c>
       <c r="F93" s="20">
-        <v>45888</v>
-      </c>
-      <c r="G93" s="20" t="s">
-        <v>86</v>
+        <v>45846</v>
+      </c>
+      <c r="G93" s="20">
+        <v>45859</v>
       </c>
       <c r="H93" s="7"/>
       <c r="I93" s="5"/>
       <c r="J93" s="5"/>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A94" s="5"/>
-      <c r="B94" s="5"/>
-      <c r="C94" s="5"/>
-      <c r="D94" s="12"/>
-      <c r="E94" s="12"/>
-      <c r="F94" s="12"/>
-      <c r="G94" s="12"/>
-      <c r="H94" s="5"/>
+    <row r="94" spans="1:10" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A94" s="18">
+        <v>33</v>
+      </c>
+      <c r="B94" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C94" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="D94" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E94" s="20">
+        <v>45862</v>
+      </c>
+      <c r="F94" s="20">
+        <v>45862</v>
+      </c>
+      <c r="G94" s="20">
+        <v>45862</v>
+      </c>
+      <c r="H94" s="7"/>
       <c r="I94" s="5"/>
       <c r="J94" s="5"/>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A95" s="5"/>
-      <c r="B95" s="5"/>
-      <c r="C95" s="5"/>
-      <c r="D95" s="12"/>
-      <c r="E95" s="12"/>
-      <c r="F95" s="12"/>
-      <c r="G95" s="12"/>
-      <c r="H95" s="5"/>
+    <row r="95" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="18">
+        <v>34</v>
+      </c>
+      <c r="B95" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C95" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D95" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E95" s="20">
+        <v>45888</v>
+      </c>
+      <c r="F95" s="20">
+        <v>45888</v>
+      </c>
+      <c r="G95" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="H95" s="7"/>
       <c r="I95" s="5"/>
       <c r="J95" s="5"/>
     </row>
-    <row r="96" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="B96" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="C96" s="33"/>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="5"/>
+      <c r="B96" s="5"/>
+      <c r="C96" s="5"/>
       <c r="D96" s="12"/>
       <c r="E96" s="12"/>
       <c r="F96" s="12"/>
@@ -3036,142 +3147,142 @@
       <c r="I97" s="5"/>
       <c r="J97" s="5"/>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A98" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B98" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C98" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D98" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E98" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="F98" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="G98" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="H98" s="6"/>
+    <row r="98" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B98" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="C98" s="33"/>
+      <c r="D98" s="12"/>
+      <c r="E98" s="12"/>
+      <c r="F98" s="12"/>
+      <c r="G98" s="12"/>
+      <c r="H98" s="5"/>
       <c r="I98" s="5"/>
       <c r="J98" s="5"/>
     </row>
-    <row r="99" spans="1:10" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="18">
-        <v>35</v>
-      </c>
-      <c r="B99" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="C99" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="D99" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="E99" s="20">
-        <v>45902</v>
-      </c>
-      <c r="F99" s="20">
-        <v>45902</v>
-      </c>
-      <c r="G99" s="20">
-        <v>45991</v>
-      </c>
-      <c r="H99" s="7"/>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="5"/>
+      <c r="B99" s="5"/>
+      <c r="C99" s="5"/>
+      <c r="D99" s="12"/>
+      <c r="E99" s="12"/>
+      <c r="F99" s="12"/>
+      <c r="G99" s="12"/>
+      <c r="H99" s="5"/>
       <c r="I99" s="5"/>
       <c r="J99" s="5"/>
     </row>
-    <row r="100" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="18">
-        <v>36</v>
-      </c>
-      <c r="B100" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="C100" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="D100" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="E100" s="20">
-        <v>45922</v>
-      </c>
-      <c r="F100" s="20">
-        <v>45901</v>
-      </c>
-      <c r="G100" s="20">
-        <v>45922</v>
-      </c>
-      <c r="H100" s="7"/>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B100" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C100" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D100" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E100" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F100" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G100" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H100" s="6"/>
       <c r="I100" s="5"/>
       <c r="J100" s="5"/>
     </row>
-    <row r="101" spans="1:10" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="18">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B101" s="18" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C101" s="19" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D101" s="25" t="s">
         <v>65</v>
       </c>
       <c r="E101" s="20">
-        <v>45923</v>
+        <v>45902</v>
       </c>
       <c r="F101" s="20">
-        <v>45923</v>
+        <v>45902</v>
       </c>
       <c r="G101" s="20">
-        <v>45935</v>
+        <v>45991</v>
       </c>
       <c r="H101" s="7"/>
       <c r="I101" s="5"/>
       <c r="J101" s="5"/>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A102" s="5"/>
-      <c r="B102" s="5"/>
-      <c r="C102" s="5"/>
-      <c r="D102" s="5"/>
-      <c r="E102" s="5"/>
-      <c r="F102" s="5"/>
-      <c r="G102" s="5"/>
-      <c r="H102" s="5"/>
+    <row r="102" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="18">
+        <v>36</v>
+      </c>
+      <c r="B102" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C102" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="D102" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E102" s="20">
+        <v>45922</v>
+      </c>
+      <c r="F102" s="20">
+        <v>45901</v>
+      </c>
+      <c r="G102" s="20">
+        <v>45922</v>
+      </c>
+      <c r="H102" s="7"/>
       <c r="I102" s="5"/>
       <c r="J102" s="5"/>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A103" s="5"/>
-      <c r="B103" s="5"/>
-      <c r="C103" s="5"/>
-      <c r="D103" s="5"/>
-      <c r="E103" s="5"/>
-      <c r="F103" s="5"/>
-      <c r="G103" s="5"/>
-      <c r="H103" s="5"/>
+    <row r="103" spans="1:10" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="18">
+        <v>37</v>
+      </c>
+      <c r="B103" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C103" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="D103" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E103" s="20">
+        <v>45923</v>
+      </c>
+      <c r="F103" s="20">
+        <v>45923</v>
+      </c>
+      <c r="G103" s="20">
+        <v>45935</v>
+      </c>
+      <c r="H103" s="7"/>
       <c r="I103" s="5"/>
       <c r="J103" s="5"/>
     </row>
-    <row r="104" spans="1:10" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A104" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="B104" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="C104" s="29"/>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" s="5"/>
+      <c r="B104" s="5"/>
+      <c r="C104" s="5"/>
       <c r="D104" s="5"/>
       <c r="E104" s="5"/>
       <c r="F104" s="5"/>
@@ -3192,87 +3303,71 @@
       <c r="I105" s="5"/>
       <c r="J105" s="5"/>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A106" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="B106" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="C106" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="D106" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E106" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="F106" s="1"/>
-      <c r="G106" s="1"/>
+    <row r="106" spans="1:10" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A106" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B106" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="C106" s="29"/>
+      <c r="D106" s="5"/>
+      <c r="E106" s="5"/>
+      <c r="F106" s="5"/>
+      <c r="G106" s="5"/>
       <c r="H106" s="5"/>
       <c r="I106" s="5"/>
       <c r="J106" s="5"/>
     </row>
-    <row r="107" spans="1:10" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A107" s="18">
-        <v>1</v>
-      </c>
-      <c r="B107" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="C107" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="D107" s="20">
-        <v>45790</v>
-      </c>
-      <c r="E107" s="20">
-        <v>45790</v>
-      </c>
-      <c r="F107" s="26"/>
-      <c r="G107" s="2"/>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107" s="5"/>
+      <c r="B107" s="5"/>
+      <c r="C107" s="5"/>
+      <c r="D107" s="5"/>
+      <c r="E107" s="5"/>
+      <c r="F107" s="5"/>
+      <c r="G107" s="5"/>
       <c r="H107" s="5"/>
       <c r="I107" s="5"/>
       <c r="J107" s="5"/>
     </row>
-    <row r="108" spans="1:10" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A108" s="18">
-        <v>2</v>
-      </c>
-      <c r="B108" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="C108" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="D108" s="20">
-        <v>45795</v>
-      </c>
-      <c r="E108" s="20">
-        <v>45797</v>
-      </c>
-      <c r="F108" s="26"/>
-      <c r="G108" s="2"/>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A108" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="B108" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="C108" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="D108" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E108" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F108" s="1"/>
+      <c r="G108" s="1"/>
       <c r="H108" s="5"/>
       <c r="I108" s="5"/>
       <c r="J108" s="5"/>
     </row>
-    <row r="109" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="18">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B109" s="18" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C109" s="19" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D109" s="20">
-        <v>45802</v>
+        <v>45790</v>
       </c>
       <c r="E109" s="20">
-        <v>45809</v>
+        <v>45790</v>
       </c>
       <c r="F109" s="26"/>
       <c r="G109" s="2"/>
@@ -3280,21 +3375,21 @@
       <c r="I109" s="5"/>
       <c r="J109" s="5"/>
     </row>
-    <row r="110" spans="1:10" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="18">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B110" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C110" s="19" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D110" s="20">
-        <v>45823</v>
+        <v>45795</v>
       </c>
       <c r="E110" s="20">
-        <v>45825</v>
+        <v>45797</v>
       </c>
       <c r="F110" s="26"/>
       <c r="G110" s="2"/>
@@ -3302,87 +3397,87 @@
       <c r="I110" s="5"/>
       <c r="J110" s="5"/>
     </row>
-    <row r="111" spans="1:10" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="18">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B111" s="18" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C111" s="19" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D111" s="20">
-        <v>45832</v>
+        <v>45802</v>
       </c>
       <c r="E111" s="20">
-        <v>45837</v>
+        <v>45809</v>
       </c>
       <c r="F111" s="26"/>
       <c r="G111" s="2"/>
-      <c r="H111" s="6"/>
+      <c r="H111" s="5"/>
       <c r="I111" s="5"/>
       <c r="J111" s="5"/>
     </row>
-    <row r="112" spans="1:10" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="18">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B112" s="18" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C112" s="19" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D112" s="20">
-        <v>45839</v>
+        <v>45823</v>
       </c>
       <c r="E112" s="20">
-        <v>45848</v>
+        <v>45825</v>
       </c>
       <c r="F112" s="26"/>
       <c r="G112" s="2"/>
-      <c r="H112" s="7"/>
+      <c r="H112" s="5"/>
       <c r="I112" s="5"/>
       <c r="J112" s="5"/>
     </row>
-    <row r="113" spans="1:10" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="18">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B113" s="18" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C113" s="19" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D113" s="20">
-        <v>45851</v>
+        <v>45832</v>
       </c>
       <c r="E113" s="20">
-        <v>45858</v>
+        <v>45837</v>
       </c>
       <c r="F113" s="26"/>
       <c r="G113" s="2"/>
-      <c r="H113" s="7"/>
+      <c r="H113" s="6"/>
       <c r="I113" s="5"/>
       <c r="J113" s="5"/>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="18">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B114" s="18" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C114" s="19" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="D114" s="20">
-        <v>45860</v>
+        <v>45839</v>
       </c>
       <c r="E114" s="20">
-        <v>45860</v>
+        <v>45848</v>
       </c>
       <c r="F114" s="26"/>
       <c r="G114" s="2"/>
@@ -3390,21 +3485,21 @@
       <c r="I114" s="5"/>
       <c r="J114" s="5"/>
     </row>
-    <row r="115" spans="1:10" ht="57" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="18">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B115" s="18" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C115" s="19" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D115" s="20">
-        <v>45872</v>
+        <v>45851</v>
       </c>
       <c r="E115" s="20">
-        <v>45881</v>
+        <v>45858</v>
       </c>
       <c r="F115" s="26"/>
       <c r="G115" s="2"/>
@@ -3412,65 +3507,65 @@
       <c r="I115" s="5"/>
       <c r="J115" s="5"/>
     </row>
-    <row r="116" spans="1:10" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="18">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B116" s="18" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C116" s="19" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="D116" s="20">
-        <v>45886</v>
+        <v>45860</v>
       </c>
       <c r="E116" s="20">
-        <v>45888</v>
+        <v>45860</v>
       </c>
       <c r="F116" s="26"/>
       <c r="G116" s="2"/>
-      <c r="H116" s="5"/>
+      <c r="H116" s="7"/>
       <c r="I116" s="5"/>
       <c r="J116" s="5"/>
     </row>
-    <row r="117" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="18">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B117" s="18" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C117" s="19" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D117" s="20">
-        <v>45893</v>
+        <v>45872</v>
       </c>
       <c r="E117" s="20">
-        <v>45902</v>
+        <v>45881</v>
       </c>
       <c r="F117" s="26"/>
       <c r="G117" s="2"/>
-      <c r="H117" s="5"/>
+      <c r="H117" s="7"/>
       <c r="I117" s="5"/>
       <c r="J117" s="5"/>
     </row>
-    <row r="118" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="18">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B118" s="18" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C118" s="19" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D118" s="20">
-        <v>45907</v>
+        <v>45886</v>
       </c>
       <c r="E118" s="20">
-        <v>45909</v>
+        <v>45888</v>
       </c>
       <c r="F118" s="26"/>
       <c r="G118" s="2"/>
@@ -3478,21 +3573,21 @@
       <c r="I118" s="5"/>
       <c r="J118" s="5"/>
     </row>
-    <row r="119" spans="1:10" ht="57" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="18">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B119" s="18" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C119" s="19" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D119" s="20">
-        <v>45916</v>
+        <v>45893</v>
       </c>
       <c r="E119" s="20">
-        <v>45923</v>
+        <v>45902</v>
       </c>
       <c r="F119" s="26"/>
       <c r="G119" s="2"/>
@@ -3500,21 +3595,21 @@
       <c r="I119" s="5"/>
       <c r="J119" s="5"/>
     </row>
-    <row r="120" spans="1:10" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="18">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B120" s="18" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C120" s="19" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D120" s="20">
-        <v>45935</v>
+        <v>45907</v>
       </c>
       <c r="E120" s="20">
-        <v>45937</v>
+        <v>45909</v>
       </c>
       <c r="F120" s="26"/>
       <c r="G120" s="2"/>
@@ -3522,60 +3617,110 @@
       <c r="I120" s="5"/>
       <c r="J120" s="5"/>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A121" s="5"/>
-      <c r="B121" s="5"/>
-      <c r="C121" s="5"/>
-      <c r="D121" s="5"/>
-      <c r="E121" s="5"/>
-      <c r="F121" s="5"/>
-      <c r="G121" s="5"/>
+    <row r="121" spans="1:10" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="18">
+        <v>14</v>
+      </c>
+      <c r="B121" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="C121" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="D121" s="20">
+        <v>45916</v>
+      </c>
+      <c r="E121" s="20">
+        <v>45923</v>
+      </c>
+      <c r="F121" s="26"/>
+      <c r="G121" s="2"/>
       <c r="H121" s="5"/>
       <c r="I121" s="5"/>
       <c r="J121" s="5"/>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A122" s="5"/>
-      <c r="B122" s="5"/>
-      <c r="C122" s="5"/>
-      <c r="D122" s="5"/>
-      <c r="E122" s="5"/>
-      <c r="F122" s="5"/>
-      <c r="G122" s="5"/>
+    <row r="122" spans="1:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="18">
+        <v>15</v>
+      </c>
+      <c r="B122" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="C122" s="38" t="s">
+        <v>127</v>
+      </c>
+      <c r="D122" s="20">
+        <v>45935</v>
+      </c>
+      <c r="E122" s="20">
+        <v>45937</v>
+      </c>
+      <c r="F122" s="26"/>
+      <c r="G122" s="2"/>
       <c r="H122" s="5"/>
       <c r="I122" s="5"/>
       <c r="J122" s="5"/>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A123" s="5"/>
-      <c r="B123" s="5"/>
-      <c r="C123" s="5"/>
-      <c r="D123" s="5"/>
-      <c r="E123" s="5"/>
+    <row r="123" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="18">
+        <v>16</v>
+      </c>
+      <c r="B123" s="39" t="s">
+        <v>140</v>
+      </c>
+      <c r="C123" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="D123" s="40">
+        <v>45949</v>
+      </c>
+      <c r="E123" s="20">
+        <v>45955</v>
+      </c>
       <c r="F123" s="5"/>
       <c r="G123" s="5"/>
       <c r="H123" s="5"/>
       <c r="I123" s="5"/>
       <c r="J123" s="5"/>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A124" s="5"/>
-      <c r="B124" s="5"/>
-      <c r="C124" s="5"/>
-      <c r="D124" s="5"/>
-      <c r="E124" s="5"/>
+    <row r="124" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="18">
+        <v>17</v>
+      </c>
+      <c r="B124" s="39" t="s">
+        <v>142</v>
+      </c>
+      <c r="C124" s="38" t="s">
+        <v>143</v>
+      </c>
+      <c r="D124" s="40">
+        <v>45956</v>
+      </c>
+      <c r="E124" s="20">
+        <v>45962</v>
+      </c>
       <c r="F124" s="5"/>
       <c r="G124" s="5"/>
       <c r="H124" s="5"/>
       <c r="I124" s="5"/>
       <c r="J124" s="5"/>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A125" s="5"/>
-      <c r="B125" s="5"/>
-      <c r="C125" s="5"/>
-      <c r="D125" s="5"/>
-      <c r="E125" s="5"/>
+    <row r="125" spans="1:10" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="18">
+        <v>18</v>
+      </c>
+      <c r="B125" s="39" t="s">
+        <v>144</v>
+      </c>
+      <c r="C125" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="D125" s="40">
+        <v>45963</v>
+      </c>
+      <c r="E125" s="20">
+        <v>45976</v>
+      </c>
       <c r="F125" s="5"/>
       <c r="G125" s="5"/>
       <c r="H125" s="5"/>
@@ -5310,72 +5455,24 @@
       <c r="I269" s="5"/>
       <c r="J269" s="5"/>
     </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A270" s="5"/>
-      <c r="B270" s="5"/>
-      <c r="C270" s="5"/>
-      <c r="D270" s="5"/>
-      <c r="E270" s="5"/>
-      <c r="F270" s="5"/>
-      <c r="G270" s="5"/>
-      <c r="H270" s="5"/>
-      <c r="I270" s="5"/>
-      <c r="J270" s="5"/>
-    </row>
-    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A271" s="5"/>
-      <c r="B271" s="5"/>
-      <c r="C271" s="5"/>
-      <c r="D271" s="5"/>
-      <c r="E271" s="5"/>
-      <c r="F271" s="5"/>
-      <c r="G271" s="5"/>
-      <c r="H271" s="5"/>
-      <c r="I271" s="5"/>
-      <c r="J271" s="5"/>
-    </row>
-    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A272" s="5"/>
-      <c r="B272" s="5"/>
-      <c r="C272" s="5"/>
-      <c r="D272" s="5"/>
-      <c r="E272" s="5"/>
-      <c r="F272" s="5"/>
-      <c r="G272" s="5"/>
-      <c r="H272" s="5"/>
-      <c r="I272" s="5"/>
-      <c r="J272" s="5"/>
-    </row>
-    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A273" s="5"/>
-      <c r="B273" s="5"/>
-      <c r="C273" s="5"/>
-      <c r="D273" s="5"/>
-      <c r="E273" s="5"/>
-      <c r="F273" s="5"/>
-      <c r="G273" s="5"/>
-      <c r="H273" s="5"/>
-      <c r="I273" s="5"/>
-      <c r="J273" s="5"/>
-    </row>
   </sheetData>
   <mergeCells count="16">
     <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="B106:C106"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="B98:C98"/>
+    <mergeCell ref="A87:B87"/>
     <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B79:C79"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>